<commit_message>
filter genes to common genes
filter genes to common genes shared by 5 dataset, before read depth normalization
</commit_message>
<xml_diff>
--- a/_summary.xlsx
+++ b/_summary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/sun_w/CAT/TCR_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wsun/research/GitHub/CAT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59D287E6-3A79-904D-A800-9EB03C113B52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E3E56DC-1C22-A748-BF27-E46F9C142BF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3480" yWindow="3380" windowWidth="28800" windowHeight="16340" xr2:uid="{D47D2F0B-AFA4-764C-A095-136D3A914E8F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="127">
   <si>
     <t>paper</t>
   </si>
@@ -410,10 +410,13 @@
     <t>GSE252432, GSE253173</t>
   </si>
   <si>
-    <t>Zheng_2021</t>
-  </si>
-  <si>
     <t>multiple cancers</t>
+  </si>
+  <si>
+    <t>Liu_2025, Zemin Zhang</t>
+  </si>
+  <si>
+    <t>Zheng_2021, Zemin Zhang</t>
   </si>
 </sst>
 </file>
@@ -831,10 +834,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71F533FF-33B4-2143-A525-77AB68BCBA13}">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -886,505 +889,542 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="E2" s="2">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>26</v>
+        <v>55</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="3">
-        <v>45675</v>
+        <v>45674</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="E3" s="2">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>19</v>
+        <v>53</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="J3" s="3">
-        <v>45675</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
       <c r="K3" s="2" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>28</v>
+        <v>71</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>29</v>
+        <v>72</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>31</v>
+        <v>74</v>
+      </c>
+      <c r="D4" t="s">
+        <v>73</v>
       </c>
       <c r="E4" s="2">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>32</v>
+        <v>75</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="3">
-        <v>45675</v>
-      </c>
-      <c r="K4" s="2"/>
+        <v>55</v>
+      </c>
+      <c r="H4" t="s">
+        <v>76</v>
+      </c>
+      <c r="J4" s="6">
+        <v>42022</v>
+      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E5" s="2">
-        <v>22</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I5" s="2"/>
-      <c r="J5" s="3">
-        <v>45674</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>37</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E6" s="2">
-        <v>13</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="I6" s="2"/>
-      <c r="J6" s="3">
-        <v>45680</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>45</v>
-      </c>
+      <c r="A6" t="s">
+        <v>126</v>
+      </c>
+      <c r="B6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E7" s="2">
-        <v>35</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>51</v>
+        <v>3</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="E8" s="2">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>53</v>
+        <v>13</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="H8" s="2"/>
+        <v>26</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
+      <c r="J8" s="3">
+        <v>45675</v>
+      </c>
       <c r="K8" s="2" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>71</v>
+        <v>16</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>72</v>
+        <v>17</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D9" t="s">
-        <v>73</v>
+        <v>18</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="E9" s="2">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>75</v>
+        <v>19</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="H9" t="s">
-        <v>76</v>
-      </c>
-      <c r="J9" s="6">
-        <v>42022</v>
+        <v>23</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J9" s="3">
+        <v>45675</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B10" t="s">
-        <v>78</v>
-      </c>
-      <c r="C10" t="s">
-        <v>79</v>
-      </c>
-      <c r="D10" t="s">
-        <v>80</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>81</v>
+        <v>28</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="G10" t="s">
-        <v>83</v>
-      </c>
-      <c r="H10" t="s">
-        <v>84</v>
-      </c>
-      <c r="J10" s="6">
+        <v>32</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="3">
         <v>45675</v>
       </c>
+      <c r="K10" s="2"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B11" t="s">
-        <v>87</v>
-      </c>
-      <c r="C11" t="s">
-        <v>86</v>
-      </c>
-      <c r="D11" t="s">
-        <v>88</v>
+        <v>40</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="E11" s="2">
-        <v>19</v>
-      </c>
-      <c r="F11" t="s">
-        <v>89</v>
-      </c>
-      <c r="G11" t="s">
-        <v>54</v>
-      </c>
-      <c r="H11" t="s">
-        <v>90</v>
-      </c>
-      <c r="J11" s="6">
-        <v>45682</v>
-      </c>
-      <c r="K11" t="s">
-        <v>91</v>
+        <v>13</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I11" s="2"/>
+      <c r="J11" s="3">
+        <v>45680</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" s="2">
+        <v>35</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B13" t="s">
+        <v>78</v>
+      </c>
+      <c r="C13" t="s">
+        <v>79</v>
+      </c>
+      <c r="D13" t="s">
+        <v>80</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G13" t="s">
+        <v>83</v>
+      </c>
+      <c r="H13" t="s">
+        <v>84</v>
+      </c>
+      <c r="J13" s="6">
+        <v>45675</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B14" t="s">
+        <v>87</v>
+      </c>
+      <c r="C14" t="s">
+        <v>86</v>
+      </c>
+      <c r="D14" t="s">
+        <v>88</v>
+      </c>
+      <c r="E14" s="2">
+        <v>19</v>
+      </c>
+      <c r="F14" t="s">
+        <v>89</v>
+      </c>
+      <c r="G14" t="s">
+        <v>54</v>
+      </c>
+      <c r="H14" t="s">
+        <v>90</v>
+      </c>
+      <c r="J14" s="6">
+        <v>45682</v>
+      </c>
+      <c r="K14" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B15" t="s">
         <v>93</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C15" t="s">
         <v>94</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D15" t="s">
         <v>116</v>
       </c>
-      <c r="E12">
+      <c r="E15">
         <v>7</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F15" t="s">
         <v>97</v>
-      </c>
-      <c r="G12" t="s">
-        <v>55</v>
-      </c>
-      <c r="H12" t="s">
-        <v>96</v>
-      </c>
-      <c r="J12" s="6">
-        <v>45675</v>
-      </c>
-      <c r="K12" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>104</v>
-      </c>
-      <c r="B13" t="s">
-        <v>105</v>
-      </c>
-      <c r="D13" t="s">
-        <v>106</v>
-      </c>
-      <c r="E13">
-        <v>38</v>
-      </c>
-      <c r="F13" t="s">
-        <v>107</v>
-      </c>
-      <c r="G13" t="s">
-        <v>108</v>
-      </c>
-      <c r="H13" t="s">
-        <v>109</v>
-      </c>
-      <c r="J13" s="6">
-        <v>45682</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>112</v>
-      </c>
-      <c r="B14" t="s">
-        <v>110</v>
-      </c>
-      <c r="C14" t="s">
-        <v>111</v>
-      </c>
-      <c r="D14" t="s">
-        <v>113</v>
-      </c>
-      <c r="E14">
-        <v>3</v>
-      </c>
-      <c r="F14" t="s">
-        <v>114</v>
-      </c>
-      <c r="H14" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>117</v>
-      </c>
-      <c r="B15" t="s">
-        <v>118</v>
-      </c>
-      <c r="C15" t="s">
-        <v>121</v>
-      </c>
-      <c r="D15" t="s">
-        <v>122</v>
-      </c>
-      <c r="E15">
-        <v>35</v>
-      </c>
-      <c r="F15" t="s">
-        <v>120</v>
       </c>
       <c r="G15" t="s">
         <v>55</v>
       </c>
       <c r="H15" t="s">
-        <v>119</v>
+        <v>96</v>
+      </c>
+      <c r="J15" s="6">
+        <v>45675</v>
+      </c>
+      <c r="K15" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>124</v>
+        <v>104</v>
       </c>
       <c r="B16" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+        <v>105</v>
+      </c>
+      <c r="D16" t="s">
+        <v>106</v>
+      </c>
+      <c r="E16">
+        <v>38</v>
+      </c>
+      <c r="F16" t="s">
+        <v>107</v>
+      </c>
+      <c r="G16" t="s">
+        <v>108</v>
+      </c>
+      <c r="H16" t="s">
+        <v>109</v>
+      </c>
+      <c r="J16" s="6">
+        <v>45682</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>112</v>
+      </c>
+      <c r="B17" t="s">
+        <v>110</v>
+      </c>
+      <c r="C17" t="s">
+        <v>111</v>
+      </c>
+      <c r="D17" t="s">
+        <v>113</v>
+      </c>
+      <c r="E17">
+        <v>3</v>
+      </c>
+      <c r="F17" t="s">
+        <v>114</v>
+      </c>
+      <c r="H17" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>117</v>
+      </c>
+      <c r="B18" t="s">
+        <v>118</v>
+      </c>
+      <c r="C18" t="s">
+        <v>121</v>
+      </c>
+      <c r="D18" t="s">
+        <v>122</v>
+      </c>
+      <c r="E18">
+        <v>35</v>
+      </c>
+      <c r="F18" t="s">
+        <v>120</v>
+      </c>
+      <c r="G18" t="s">
+        <v>55</v>
+      </c>
+      <c r="H18" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>57</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B24" t="s">
         <v>58</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C24" t="s">
         <v>59</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D24" t="s">
         <v>60</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E24" t="s">
         <v>61</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="F24" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="H21" s="5" t="s">
+      <c r="H24" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="K21" s="2" t="s">
+      <c r="K24" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>66</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B25" t="s">
         <v>67</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C25" t="s">
         <v>68</v>
       </c>
-      <c r="E22">
+      <c r="E25">
         <v>2</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="F25" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="K22" t="s">
+      <c r="K25" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>98</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B26" t="s">
         <v>34</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C26" t="s">
         <v>99</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D26" t="s">
         <v>100</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E26" t="s">
         <v>102</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F26" t="s">
         <v>101</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G26" t="s">
         <v>55</v>
       </c>
-      <c r="K23" t="s">
+      <c r="K26" t="s">
         <v>103</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I3" r:id="rId1" xr:uid="{0CBC73CE-FBEB-1747-B55F-20D1BEB1D7BE}"/>
+    <hyperlink ref="I9" r:id="rId1" xr:uid="{0CBC73CE-FBEB-1747-B55F-20D1BEB1D7BE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>